<commit_message>
Making Maps of Catchment Areas for Hospitals, Timeline based on when Hospitals' Open/Close Status Doesn't Change, Heat Map of Attacks during Timeline layered over.
</commit_message>
<xml_diff>
--- a/Hospitals_OpenCloseoverTime.xlsx
+++ b/Hospitals_OpenCloseoverTime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctr22\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3dbe731901b40241/Desktop/Monona Zhou/bassproj/BassConnectionsFireinmysoul/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA290550-84C0-4775-84F1-03436318159C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{CA290550-84C0-4775-84F1-03436318159C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D02DEBC3-B6BC-4C79-9DD7-8F74C5E3694B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FBA0BD12-E686-4212-82D9-88D5B27688C0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{FBA0BD12-E686-4212-82D9-88D5B27688C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -143,6 +143,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -465,21 +469,21 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -531,7 +535,7 @@
         <v>31.523690930000001</v>
       </c>
       <c r="D2" s="3">
-        <v>45200</v>
+        <v>45206</v>
       </c>
       <c r="E2" s="3">
         <v>45253</v>
@@ -550,7 +554,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -561,7 +565,7 @@
         <v>31.505609400000001</v>
       </c>
       <c r="D3" s="3">
-        <v>45200</v>
+        <v>45206</v>
       </c>
       <c r="E3" s="3">
         <v>45235</v>
@@ -576,7 +580,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -587,7 +591,7 @@
         <v>31.34689036</v>
       </c>
       <c r="D4" s="3">
-        <v>45200</v>
+        <v>45206</v>
       </c>
       <c r="E4" s="3">
         <v>45342</v>
@@ -602,7 +606,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -613,7 +617,7 @@
         <v>31.303173999999999</v>
       </c>
       <c r="D5" s="3">
-        <v>45200</v>
+        <v>45206</v>
       </c>
       <c r="E5" s="3">
         <v>45474</v>
@@ -628,7 +632,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -639,7 +643,7 @@
         <v>31.288121889999999</v>
       </c>
       <c r="D6" s="3">
-        <v>45200</v>
+        <v>45206</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>

</xml_diff>